<commit_message>
Modified Excel spreadsheet file
</commit_message>
<xml_diff>
--- a/African Marigold Data Analysis.xlsx
+++ b/African Marigold Data Analysis.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="60">
   <si>
     <t xml:space="preserve">Height (cm) </t>
   </si>
@@ -412,12 +412,27 @@
     <t>Table 6. Negative Control Group: Summary of Table 3
  No fertilization treatment.</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">LINK TO REPO: </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://github.com/CSjianbel/African-Marigold-Analysis</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -467,11 +482,8 @@
       <sz val="10.0"/>
     </font>
     <font>
-      <sz val="10.0"/>
-    </font>
-    <font>
-      <b/>
-      <name val="Arial"/>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="3">
@@ -599,7 +611,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="72">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -698,10 +710,7 @@
     <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -710,10 +719,7 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="10" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="11" numFmtId="11" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -756,7 +762,7 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="11" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -768,10 +774,7 @@
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -796,9 +799,6 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -807,6 +807,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -832,7 +838,7 @@
     <xdr:ext cx="7162800" cy="2609850"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -860,7 +866,7 @@
     <xdr:ext cx="7162800" cy="2609850"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -888,7 +894,7 @@
     <xdr:ext cx="7162800" cy="2609850"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -944,7 +950,7 @@
     <xdr:ext cx="7162800" cy="2609850"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -972,7 +978,7 @@
     <xdr:ext cx="7162800" cy="2609850"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1956,22 +1962,22 @@
       <c r="N5" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="P5" s="33" t="s">
+      <c r="P5" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="Q5" s="33" t="s">
+      <c r="Q5" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="R5" s="33" t="s">
+      <c r="R5" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="S5" s="33" t="s">
+      <c r="S5" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="T5" s="33" t="s">
+      <c r="T5" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="U5" s="33" t="s">
+      <c r="U5" s="32" t="s">
         <v>33</v>
       </c>
       <c r="V5" s="33" t="s">
@@ -2025,25 +2031,25 @@
       <c r="Q6" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="R6" s="37">
+      <c r="R6" s="35">
         <v>-21.6667</v>
       </c>
-      <c r="S6" s="37">
+      <c r="S6" s="35">
         <v>0.001</v>
       </c>
-      <c r="T6" s="37">
+      <c r="T6" s="35">
         <v>-28.1169</v>
       </c>
-      <c r="U6" s="37">
+      <c r="U6" s="35">
         <v>-15.2164</v>
       </c>
-      <c r="V6" s="37" t="b">
+      <c r="V6" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="W6" s="38"/>
-      <c r="X6" s="38"/>
-      <c r="Y6" s="38"/>
-      <c r="Z6" s="38"/>
+      <c r="W6" s="37"/>
+      <c r="X6" s="37"/>
+      <c r="Y6" s="37"/>
+      <c r="Z6" s="37"/>
     </row>
     <row r="7">
       <c r="A7" s="25">
@@ -2058,7 +2064,7 @@
       <c r="D7" s="26">
         <v>374.0</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="38" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="30">
@@ -2088,25 +2094,25 @@
       <c r="Q7" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="R7" s="37">
+      <c r="R7" s="35">
         <v>-6.5</v>
       </c>
-      <c r="S7" s="37">
+      <c r="S7" s="35">
         <v>0.0479</v>
       </c>
-      <c r="T7" s="37">
+      <c r="T7" s="35">
         <v>-12.9503</v>
       </c>
-      <c r="U7" s="37">
+      <c r="U7" s="35">
         <v>-0.0497</v>
       </c>
-      <c r="V7" s="37" t="b">
+      <c r="V7" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="W7" s="38"/>
-      <c r="X7" s="38"/>
-      <c r="Y7" s="38"/>
-      <c r="Z7" s="38"/>
+      <c r="W7" s="37"/>
+      <c r="X7" s="37"/>
+      <c r="Y7" s="37"/>
+      <c r="Z7" s="37"/>
     </row>
     <row r="8">
       <c r="A8" s="25">
@@ -2121,7 +2127,7 @@
       <c r="D8" s="26">
         <v>310.0</v>
       </c>
-      <c r="F8" s="39">
+      <c r="F8" s="38">
         <v>0.25</v>
       </c>
       <c r="G8" s="30">
@@ -2139,28 +2145,28 @@
       <c r="P8" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="40" t="s">
+      <c r="Q8" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="R8" s="41">
+      <c r="R8" s="34">
         <v>15.1667</v>
       </c>
-      <c r="S8" s="37">
+      <c r="S8" s="35">
         <v>0.001</v>
       </c>
-      <c r="T8" s="37">
+      <c r="T8" s="35">
         <v>8.7164</v>
       </c>
-      <c r="U8" s="37">
+      <c r="U8" s="35">
         <v>21.6169</v>
       </c>
-      <c r="V8" s="37" t="b">
+      <c r="V8" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="W8" s="38"/>
-      <c r="X8" s="38"/>
-      <c r="Y8" s="38"/>
-      <c r="Z8" s="38"/>
+      <c r="W8" s="37"/>
+      <c r="X8" s="37"/>
+      <c r="Y8" s="37"/>
+      <c r="Z8" s="37"/>
     </row>
     <row r="9">
       <c r="A9" s="25">
@@ -2175,7 +2181,7 @@
       <c r="D9" s="26">
         <v>414.0</v>
       </c>
-      <c r="F9" s="39">
+      <c r="F9" s="38">
         <v>0.5</v>
       </c>
       <c r="G9" s="30">
@@ -2190,10 +2196,10 @@
       <c r="K9" s="22"/>
       <c r="L9" s="22"/>
       <c r="M9" s="22"/>
-      <c r="P9" s="42"/>
-      <c r="Q9" s="43"/>
-      <c r="R9" s="44"/>
-      <c r="S9" s="42"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="41"/>
+      <c r="R9" s="42"/>
+      <c r="S9" s="40"/>
     </row>
     <row r="10">
       <c r="A10" s="25">
@@ -2208,7 +2214,7 @@
       <c r="D10" s="26">
         <v>386.0</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10" s="38">
         <v>0.75</v>
       </c>
       <c r="G10" s="30">
@@ -2244,7 +2250,7 @@
       <c r="D11" s="26">
         <v>366.0</v>
       </c>
-      <c r="F11" s="45" t="s">
+      <c r="F11" s="43" t="s">
         <v>37</v>
       </c>
       <c r="G11" s="30">
@@ -2259,22 +2265,22 @@
       <c r="K11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P11" s="33" t="s">
+      <c r="P11" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="Q11" s="33" t="s">
+      <c r="Q11" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="R11" s="33" t="s">
+      <c r="R11" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="S11" s="33" t="s">
+      <c r="S11" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="T11" s="33" t="s">
+      <c r="T11" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="U11" s="33" t="s">
+      <c r="U11" s="32" t="s">
         <v>33</v>
       </c>
       <c r="V11" s="33" t="s">
@@ -2304,25 +2310,25 @@
       <c r="Q12" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="R12" s="37">
+      <c r="R12" s="35">
         <v>-9.25</v>
       </c>
-      <c r="S12" s="37">
+      <c r="S12" s="35">
         <v>0.0078</v>
       </c>
-      <c r="T12" s="37">
+      <c r="T12" s="35">
         <v>-16.2868</v>
       </c>
-      <c r="U12" s="37">
+      <c r="U12" s="35">
         <v>-2.2132</v>
       </c>
-      <c r="V12" s="37" t="b">
+      <c r="V12" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="W12" s="38"/>
-      <c r="X12" s="38"/>
-      <c r="Y12" s="38"/>
-      <c r="Z12" s="38"/>
+      <c r="W12" s="37"/>
+      <c r="X12" s="37"/>
+      <c r="Y12" s="37"/>
+      <c r="Z12" s="37"/>
     </row>
     <row r="13">
       <c r="A13" s="25">
@@ -2343,39 +2349,39 @@
       <c r="L13" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="M13" s="46" t="s">
+      <c r="M13" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="N13" s="47">
+      <c r="N13" s="45">
         <f> 0.05 / 3</f>
         <v>0.01666666667</v>
       </c>
-      <c r="O13" s="47"/>
+      <c r="O13" s="45"/>
       <c r="P13" s="36" t="s">
         <v>4</v>
       </c>
       <c r="Q13" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="R13" s="37">
+      <c r="R13" s="35">
         <v>-12.3333</v>
       </c>
-      <c r="S13" s="37">
+      <c r="S13" s="35">
         <v>0.001</v>
       </c>
-      <c r="T13" s="37">
+      <c r="T13" s="35">
         <v>-19.3702</v>
       </c>
-      <c r="U13" s="37">
+      <c r="U13" s="35">
         <v>-5.2965</v>
       </c>
-      <c r="V13" s="37" t="b">
+      <c r="V13" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="W13" s="38"/>
-      <c r="X13" s="38"/>
-      <c r="Y13" s="38"/>
-      <c r="Z13" s="38"/>
+      <c r="W13" s="37"/>
+      <c r="X13" s="37"/>
+      <c r="Y13" s="37"/>
+      <c r="Z13" s="37"/>
     </row>
     <row r="14">
       <c r="A14" s="25">
@@ -2396,25 +2402,25 @@
       <c r="Q14" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="R14" s="41">
+      <c r="R14" s="34">
         <v>-3.0833</v>
       </c>
-      <c r="S14" s="37">
+      <c r="S14" s="35">
         <v>0.5351</v>
       </c>
-      <c r="T14" s="37">
+      <c r="T14" s="35">
         <v>-10.1202</v>
       </c>
-      <c r="U14" s="37">
+      <c r="U14" s="35">
         <v>3.9535</v>
       </c>
-      <c r="V14" s="37" t="b">
+      <c r="V14" s="35" t="b">
         <v>0</v>
       </c>
-      <c r="W14" s="38"/>
-      <c r="X14" s="38"/>
-      <c r="Y14" s="38"/>
-      <c r="Z14" s="38"/>
+      <c r="W14" s="37"/>
+      <c r="X14" s="37"/>
+      <c r="Y14" s="37"/>
+      <c r="Z14" s="37"/>
     </row>
     <row r="15">
       <c r="K15" s="6" t="s">
@@ -2422,10 +2428,10 @@
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="2"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="43"/>
-      <c r="R15" s="44"/>
-      <c r="S15" s="42"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="41"/>
+      <c r="R15" s="42"/>
+      <c r="S15" s="40"/>
     </row>
     <row r="16">
       <c r="K16" s="1" t="s">
@@ -2435,7 +2441,7 @@
         <v>7</v>
       </c>
       <c r="M16" s="2"/>
-      <c r="N16" s="48"/>
+      <c r="N16" s="46"/>
       <c r="P16" s="2" t="s">
         <v>43</v>
       </c>
@@ -2452,23 +2458,23 @@
         <v>9</v>
       </c>
       <c r="M17" s="2"/>
-      <c r="N17" s="49"/>
-      <c r="P17" s="33" t="s">
+      <c r="N17" s="47"/>
+      <c r="P17" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="Q17" s="33" t="s">
+      <c r="Q17" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="R17" s="33" t="s">
+      <c r="R17" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="S17" s="33" t="s">
+      <c r="S17" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="T17" s="33" t="s">
+      <c r="T17" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="U17" s="33" t="s">
+      <c r="U17" s="32" t="s">
         <v>33</v>
       </c>
       <c r="V17" s="33" t="s">
@@ -2496,32 +2502,32 @@
         <v>11</v>
       </c>
       <c r="M18" s="2"/>
-      <c r="N18" s="48"/>
+      <c r="N18" s="46"/>
       <c r="P18" s="36" t="s">
         <v>4</v>
       </c>
       <c r="Q18" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="R18" s="37">
+      <c r="R18" s="35">
         <v>-112.3333</v>
       </c>
-      <c r="S18" s="37">
+      <c r="S18" s="35">
         <v>0.001</v>
       </c>
-      <c r="T18" s="37">
+      <c r="T18" s="35">
         <v>-154.9302</v>
       </c>
-      <c r="U18" s="37">
+      <c r="U18" s="35">
         <v>-69.7365</v>
       </c>
-      <c r="V18" s="37" t="b">
+      <c r="V18" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="W18" s="38"/>
-      <c r="X18" s="38"/>
-      <c r="Y18" s="38"/>
-      <c r="Z18" s="38"/>
+      <c r="W18" s="37"/>
+      <c r="X18" s="37"/>
+      <c r="Y18" s="37"/>
+      <c r="Z18" s="37"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
@@ -2543,25 +2549,25 @@
       <c r="Q19" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="R19" s="37">
+      <c r="R19" s="35">
         <v>-79.4167</v>
       </c>
-      <c r="S19" s="37">
+      <c r="S19" s="35">
         <v>0.001</v>
       </c>
-      <c r="T19" s="37">
+      <c r="T19" s="35">
         <v>-122.0135</v>
       </c>
-      <c r="U19" s="37">
+      <c r="U19" s="35">
         <v>-36.8198</v>
       </c>
-      <c r="V19" s="37" t="b">
+      <c r="V19" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="W19" s="38"/>
-      <c r="X19" s="38"/>
-      <c r="Y19" s="38"/>
-      <c r="Z19" s="38"/>
+      <c r="W19" s="37"/>
+      <c r="X19" s="37"/>
+      <c r="Y19" s="37"/>
+      <c r="Z19" s="37"/>
     </row>
     <row r="20">
       <c r="A20" s="25">
@@ -2576,7 +2582,7 @@
       <c r="D20" s="26">
         <v>235.0</v>
       </c>
-      <c r="F20" s="50"/>
+      <c r="F20" s="48"/>
       <c r="G20" s="32" t="s">
         <v>20</v>
       </c>
@@ -2586,7 +2592,7 @@
       <c r="I20" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="K20" s="51" t="s">
+      <c r="K20" s="49" t="s">
         <v>48</v>
       </c>
       <c r="P20" s="36" t="s">
@@ -2595,25 +2601,25 @@
       <c r="Q20" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="R20" s="37">
+      <c r="R20" s="35">
         <v>32.9167</v>
       </c>
-      <c r="S20" s="37">
+      <c r="S20" s="35">
         <v>0.1559</v>
       </c>
-      <c r="T20" s="37">
+      <c r="T20" s="35">
         <v>-9.6802</v>
       </c>
-      <c r="U20" s="37">
+      <c r="U20" s="35">
         <v>75.5135</v>
       </c>
-      <c r="V20" s="37" t="b">
+      <c r="V20" s="35" t="b">
         <v>0</v>
       </c>
-      <c r="W20" s="38"/>
-      <c r="X20" s="38"/>
-      <c r="Y20" s="38"/>
-      <c r="Z20" s="38"/>
+      <c r="W20" s="37"/>
+      <c r="X20" s="37"/>
+      <c r="Y20" s="37"/>
+      <c r="Z20" s="37"/>
     </row>
     <row r="21">
       <c r="A21" s="25">
@@ -2631,31 +2637,31 @@
       <c r="F21" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="52">
+      <c r="G21" s="50">
         <v>12.0</v>
       </c>
-      <c r="H21" s="52">
+      <c r="H21" s="50">
         <v>12.0</v>
       </c>
-      <c r="I21" s="52">
+      <c r="I21" s="50">
         <v>12.0</v>
       </c>
-      <c r="K21" s="53" t="s">
+      <c r="K21" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="L21" s="54" t="s">
+      <c r="L21" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="M21" s="55" t="s">
+      <c r="M21" s="53" t="s">
         <v>24</v>
       </c>
       <c r="N21" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="P21" s="42"/>
-      <c r="Q21" s="43"/>
-      <c r="R21" s="44"/>
-      <c r="S21" s="42"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="42"/>
+      <c r="S21" s="40"/>
     </row>
     <row r="22">
       <c r="A22" s="25">
@@ -2673,33 +2679,33 @@
       <c r="F22" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="52">
+      <c r="G22" s="50">
         <v>64.0</v>
       </c>
-      <c r="H22" s="52">
+      <c r="H22" s="50">
         <v>31.1666666666667</v>
       </c>
-      <c r="I22" s="52">
+      <c r="I22" s="50">
         <v>280.083333333333</v>
       </c>
-      <c r="K22" s="56" t="s">
+      <c r="K22" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="L22" s="57">
+      <c r="L22" s="55">
         <v>2.71785852591474</v>
       </c>
-      <c r="M22" s="58">
+      <c r="M22" s="56">
         <v>0.012564279857587</v>
       </c>
-      <c r="N22" s="59" t="b">
+      <c r="N22" s="57" t="b">
         <v>1</v>
       </c>
-      <c r="P22" s="60" t="s">
+      <c r="P22" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="Q22" s="43"/>
-      <c r="R22" s="44"/>
-      <c r="S22" s="42"/>
+      <c r="Q22" s="41"/>
+      <c r="R22" s="42"/>
+      <c r="S22" s="40"/>
     </row>
     <row r="23">
       <c r="A23" s="25">
@@ -2717,31 +2723,31 @@
       <c r="F23" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="52">
+      <c r="G23" s="50">
         <v>6.09023062707063</v>
       </c>
-      <c r="H23" s="52">
+      <c r="H23" s="50">
         <v>8.57939745005794</v>
       </c>
-      <c r="I23" s="52">
+      <c r="I23" s="50">
         <v>49.0703730895896</v>
       </c>
-      <c r="K23" s="56" t="s">
+      <c r="K23" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="L23" s="57">
+      <c r="L23" s="55">
         <v>8.0314268217978</v>
       </c>
-      <c r="M23" s="58">
+      <c r="M23" s="56">
         <v>5.53092858862259E-8</v>
       </c>
-      <c r="N23" s="59" t="b">
+      <c r="N23" s="57" t="b">
         <v>1</v>
       </c>
-      <c r="P23" s="42"/>
-      <c r="Q23" s="43"/>
-      <c r="R23" s="44"/>
-      <c r="S23" s="42"/>
+      <c r="P23" s="40"/>
+      <c r="Q23" s="41"/>
+      <c r="R23" s="42"/>
+      <c r="S23" s="40"/>
     </row>
     <row r="24">
       <c r="A24" s="25">
@@ -2759,25 +2765,25 @@
       <c r="F24" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="52">
+      <c r="G24" s="50">
         <v>58.0</v>
       </c>
-      <c r="H24" s="52">
+      <c r="H24" s="50">
         <v>21.0</v>
       </c>
-      <c r="I24" s="52">
+      <c r="I24" s="50">
         <v>207.0</v>
       </c>
-      <c r="K24" s="61" t="s">
+      <c r="K24" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="L24" s="57">
+      <c r="L24" s="55">
         <v>5.45158132917237</v>
       </c>
-      <c r="M24" s="58">
+      <c r="M24" s="56">
         <v>1.77815781034481E-5</v>
       </c>
-      <c r="N24" s="62" t="b">
+      <c r="N24" s="59" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2794,22 +2800,22 @@
       <c r="D25" s="26">
         <v>250.0</v>
       </c>
-      <c r="F25" s="63">
+      <c r="F25" s="60">
         <v>0.25</v>
       </c>
-      <c r="G25" s="52">
+      <c r="G25" s="50">
         <v>58.0</v>
       </c>
-      <c r="H25" s="52">
+      <c r="H25" s="50">
         <v>26.75</v>
       </c>
-      <c r="I25" s="52">
+      <c r="I25" s="50">
         <v>249.75</v>
       </c>
-      <c r="K25" s="64"/>
-      <c r="L25" s="64"/>
-      <c r="M25" s="64"/>
-      <c r="N25" s="64"/>
+      <c r="K25" s="61"/>
+      <c r="L25" s="61"/>
+      <c r="M25" s="61"/>
+      <c r="N25" s="61"/>
     </row>
     <row r="26">
       <c r="A26" s="25">
@@ -2824,24 +2830,24 @@
       <c r="D26" s="26">
         <v>293.0</v>
       </c>
-      <c r="F26" s="63">
+      <c r="F26" s="60">
         <v>0.5</v>
       </c>
-      <c r="G26" s="52">
+      <c r="G26" s="50">
         <v>62.5</v>
       </c>
-      <c r="H26" s="52">
+      <c r="H26" s="50">
         <v>28.5</v>
       </c>
-      <c r="I26" s="52">
+      <c r="I26" s="50">
         <v>273.5</v>
       </c>
-      <c r="K26" s="65" t="s">
+      <c r="K26" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="L26" s="66"/>
-      <c r="M26" s="66"/>
-      <c r="N26" s="66"/>
+      <c r="L26" s="63"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="63"/>
     </row>
     <row r="27">
       <c r="A27" s="25">
@@ -2856,25 +2862,25 @@
       <c r="D27" s="26">
         <v>260.0</v>
       </c>
-      <c r="F27" s="63">
+      <c r="F27" s="60">
         <v>0.75</v>
       </c>
-      <c r="G27" s="52">
+      <c r="G27" s="50">
         <v>70.0</v>
       </c>
-      <c r="H27" s="52">
+      <c r="H27" s="50">
         <v>31.25</v>
       </c>
-      <c r="I27" s="52">
+      <c r="I27" s="50">
         <v>299.25</v>
       </c>
-      <c r="K27" s="56" t="s">
+      <c r="K27" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="L27" s="67" t="s">
+      <c r="L27" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="M27" s="68" t="s">
+      <c r="M27" s="65" t="s">
         <v>24</v>
       </c>
       <c r="N27" s="33" t="s">
@@ -2897,25 +2903,25 @@
       <c r="F28" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="G28" s="52">
+      <c r="G28" s="50">
         <v>72.0</v>
       </c>
-      <c r="H28" s="52">
+      <c r="H28" s="50">
         <v>52.0</v>
       </c>
-      <c r="I28" s="52">
+      <c r="I28" s="50">
         <v>394.0</v>
       </c>
-      <c r="K28" s="56" t="s">
+      <c r="K28" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="L28" s="57">
+      <c r="L28" s="55">
         <v>4.1809062157238</v>
       </c>
-      <c r="M28" s="58">
+      <c r="M28" s="56">
         <v>3.87874830903E-4</v>
       </c>
-      <c r="N28" s="59" t="b">
+      <c r="N28" s="57" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2932,16 +2938,16 @@
       <c r="D29" s="26">
         <v>265.0</v>
       </c>
-      <c r="K29" s="56" t="s">
+      <c r="K29" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="L29" s="57">
+      <c r="L29" s="55">
         <v>3.71296173339954</v>
       </c>
-      <c r="M29" s="58">
+      <c r="M29" s="56">
         <v>0.001211479431689</v>
       </c>
-      <c r="N29" s="59" t="b">
+      <c r="N29" s="57" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2958,16 +2964,16 @@
       <c r="D30" s="26">
         <v>394.0</v>
       </c>
-      <c r="K30" s="61" t="s">
+      <c r="K30" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="L30" s="57">
+      <c r="L30" s="55">
         <v>-0.986339933411334</v>
       </c>
-      <c r="M30" s="58">
+      <c r="M30" s="56">
         <v>0.334690659752219</v>
       </c>
-      <c r="N30" s="62" t="b">
+      <c r="N30" s="59" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2984,33 +2990,33 @@
       <c r="D31" s="26">
         <v>282.0</v>
       </c>
-      <c r="K31" s="69"/>
-      <c r="L31" s="69"/>
-      <c r="M31" s="69"/>
-      <c r="N31" s="69"/>
+      <c r="K31" s="66"/>
+      <c r="L31" s="66"/>
+      <c r="M31" s="66"/>
+      <c r="N31" s="66"/>
     </row>
     <row r="32">
-      <c r="K32" s="64"/>
-      <c r="L32" s="64"/>
-      <c r="M32" s="64"/>
-      <c r="N32" s="64"/>
+      <c r="K32" s="61"/>
+      <c r="L32" s="61"/>
+      <c r="M32" s="61"/>
+      <c r="N32" s="61"/>
     </row>
     <row r="33">
-      <c r="K33" s="65" t="s">
+      <c r="K33" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="L33" s="66"/>
-      <c r="M33" s="66"/>
-      <c r="N33" s="66"/>
+      <c r="L33" s="63"/>
+      <c r="M33" s="63"/>
+      <c r="N33" s="63"/>
     </row>
     <row r="34">
-      <c r="K34" s="70" t="s">
+      <c r="K34" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="L34" s="71" t="s">
+      <c r="L34" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="M34" s="68" t="s">
+      <c r="M34" s="65" t="s">
         <v>24</v>
       </c>
       <c r="N34" s="33" t="s">
@@ -3027,16 +3033,16 @@
       <c r="F35" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K35" s="56" t="s">
+      <c r="K35" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="L35" s="57">
+      <c r="L35" s="55">
         <v>4.1809062157238</v>
       </c>
-      <c r="M35" s="58">
+      <c r="M35" s="56">
         <v>3.87874830903E-4</v>
       </c>
-      <c r="N35" s="59" t="b">
+      <c r="N35" s="57" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3053,16 +3059,16 @@
       <c r="D36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K36" s="56" t="s">
+      <c r="K36" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="L36" s="57">
+      <c r="L36" s="55">
         <v>3.71296173339954</v>
       </c>
-      <c r="M36" s="58">
+      <c r="M36" s="56">
         <v>0.001211479431689</v>
       </c>
-      <c r="N36" s="59" t="b">
+      <c r="N36" s="57" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3079,7 +3085,7 @@
       <c r="D37" s="26">
         <v>227.0</v>
       </c>
-      <c r="F37" s="72"/>
+      <c r="F37" s="68"/>
       <c r="G37" s="32" t="s">
         <v>20</v>
       </c>
@@ -3089,16 +3095,16 @@
       <c r="I37" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="K37" s="61" t="s">
+      <c r="K37" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="L37" s="57">
+      <c r="L37" s="55">
         <v>-0.986339933411334</v>
       </c>
-      <c r="M37" s="58">
+      <c r="M37" s="56">
         <v>0.334690659752219</v>
       </c>
-      <c r="N37" s="62" t="b">
+      <c r="N37" s="59" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3118,13 +3124,13 @@
       <c r="F38" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="G38" s="52">
+      <c r="G38" s="50">
         <v>12.0</v>
       </c>
-      <c r="H38" s="52">
+      <c r="H38" s="50">
         <v>12.0</v>
       </c>
-      <c r="I38" s="52">
+      <c r="I38" s="50">
         <v>12.0</v>
       </c>
     </row>
@@ -3144,13 +3150,13 @@
       <c r="F39" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="G39" s="52">
+      <c r="G39" s="50">
         <v>48.8333333333333</v>
       </c>
-      <c r="H39" s="52">
+      <c r="H39" s="50">
         <v>34.25</v>
       </c>
-      <c r="I39" s="52">
+      <c r="I39" s="50">
         <v>247.166666666667</v>
       </c>
     </row>
@@ -3170,13 +3176,13 @@
       <c r="F40" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="G40" s="52">
+      <c r="G40" s="50">
         <v>7.46912838207235</v>
       </c>
-      <c r="H40" s="52">
+      <c r="H40" s="50">
         <v>6.60750262270783</v>
       </c>
-      <c r="I40" s="52">
+      <c r="I40" s="50">
         <v>37.8125360004837</v>
       </c>
     </row>
@@ -3196,13 +3202,13 @@
       <c r="F41" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="G41" s="52">
+      <c r="G41" s="50">
         <v>36.0</v>
       </c>
-      <c r="H41" s="52">
+      <c r="H41" s="50">
         <v>23.0</v>
       </c>
-      <c r="I41" s="52">
+      <c r="I41" s="50">
         <v>192.0</v>
       </c>
     </row>
@@ -3219,16 +3225,16 @@
       <c r="D42" s="26">
         <v>192.0</v>
       </c>
-      <c r="F42" s="63">
+      <c r="F42" s="60">
         <v>0.25</v>
       </c>
-      <c r="G42" s="52">
+      <c r="G42" s="50">
         <v>44.75</v>
       </c>
-      <c r="H42" s="52">
+      <c r="H42" s="50">
         <v>29.0</v>
       </c>
-      <c r="I42" s="52">
+      <c r="I42" s="50">
         <v>224.25</v>
       </c>
     </row>
@@ -3245,16 +3251,16 @@
       <c r="D43" s="26">
         <v>275.0</v>
       </c>
-      <c r="F43" s="63">
+      <c r="F43" s="60">
         <v>0.5</v>
       </c>
-      <c r="G43" s="52">
+      <c r="G43" s="50">
         <v>47.5</v>
       </c>
-      <c r="H43" s="52">
+      <c r="H43" s="50">
         <v>37.0</v>
       </c>
-      <c r="I43" s="52">
+      <c r="I43" s="50">
         <v>240.0</v>
       </c>
     </row>
@@ -3271,16 +3277,16 @@
       <c r="D44" s="26">
         <v>244.0</v>
       </c>
-      <c r="F44" s="63">
+      <c r="F44" s="60">
         <v>0.75</v>
       </c>
-      <c r="G44" s="52">
+      <c r="G44" s="50">
         <v>52.25</v>
       </c>
-      <c r="H44" s="52">
+      <c r="H44" s="50">
         <v>39.0</v>
       </c>
-      <c r="I44" s="52">
+      <c r="I44" s="50">
         <v>275.25</v>
       </c>
     </row>
@@ -3300,13 +3306,13 @@
       <c r="F45" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="G45" s="52">
+      <c r="G45" s="50">
         <v>64.0</v>
       </c>
-      <c r="H45" s="52">
+      <c r="H45" s="50">
         <v>42.0</v>
       </c>
-      <c r="I45" s="52">
+      <c r="I45" s="50">
         <v>326.0</v>
       </c>
     </row>
@@ -3364,26 +3370,26 @@
       <c r="A52" s="29"/>
       <c r="B52" s="29"/>
       <c r="F52" s="29"/>
-      <c r="G52" s="73"/>
+      <c r="G52" s="69"/>
       <c r="H52" s="22"/>
     </row>
     <row r="53">
       <c r="A53" s="29"/>
-      <c r="B53" s="73"/>
+      <c r="B53" s="69"/>
       <c r="F53" s="29"/>
-      <c r="G53" s="73"/>
+      <c r="G53" s="69"/>
       <c r="H53" s="22"/>
     </row>
     <row r="54">
       <c r="A54" s="29"/>
-      <c r="B54" s="73"/>
+      <c r="B54" s="69"/>
       <c r="F54" s="29"/>
-      <c r="G54" s="73"/>
+      <c r="G54" s="69"/>
       <c r="H54" s="22"/>
     </row>
     <row r="55">
       <c r="A55" s="29"/>
-      <c r="B55" s="73"/>
+      <c r="B55" s="69"/>
       <c r="F55" s="22"/>
       <c r="G55" s="22"/>
       <c r="H55" s="22"/>
@@ -3397,16 +3403,23 @@
       <c r="F57" s="22"/>
       <c r="G57" s="22"/>
       <c r="H57" s="22"/>
+    </row>
+    <row r="67">
+      <c r="P67" s="70" t="s">
+        <v>59</v>
+      </c>
+      <c r="S67" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="K2:L2"/>
+    <mergeCell ref="P2:V2"/>
     <mergeCell ref="P3:T3"/>
-    <mergeCell ref="P2:V2"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="P10:V10"/>
+    <mergeCell ref="K20:N20"/>
     <mergeCell ref="K26:N26"/>
     <mergeCell ref="K33:N33"/>
     <mergeCell ref="A35:D35"/>
@@ -3414,12 +3427,14 @@
     <mergeCell ref="K11:N11"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="M15:N15"/>
+    <mergeCell ref="P16:V16"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="K19:N19"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="P16:V16"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="P67"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified Excel Spreadsheet : Added Summary of Analysis
</commit_message>
<xml_diff>
--- a/African Marigold Data Analysis.xlsx
+++ b/African Marigold Data Analysis.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="62">
   <si>
     <t xml:space="preserve">Height (cm) </t>
   </si>
@@ -257,7 +257,7 @@
     </r>
   </si>
   <si>
-    <t>Table 13 Determine Significant Differences of the Total length of leaves (cm) between fertilization treatments through Tukey’s Honest Significant Difference.</t>
+    <t>Table 13. Determine Significant Differences of the Total length of leaves (cm) between fertilization treatments through Tukey’s Honest Significant Difference.</t>
   </si>
   <si>
     <r>
@@ -413,6 +413,36 @@
  No fertilization treatment.</t>
   </si>
   <si>
+    <t>Summary of Analysis:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">The results of One-Way Anova test for each of the growth paramaters had p-values that were all less than or equal to </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>alpha</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>. This concludes that there exists significant differences between the groups for each of the growth parameters. We now have reason to believe that a significant difference between the groups exist, therefore another question may now be answered which is where does the significant differences lie. 2 Post-Hoc methods were utilised to find the significant differences. Firstly the Bonferroni Test which is to just do t-tests between each possible pairs of each data group. Though performing multiple t-tests can cause randomness, to adjust for this we correct our significance level by, alpha / no. of pairs. After performing Bonferroni Test the results show that each fertilization treatment has significant differences with each other, for each growth parameter. Except for the Positive Control Group and the Negative Control Group as they had no significant differences in the number of leaves and total length of leaves (cm) growth parameters. Merely for verification the Tukey’s Honest Significant Difference were also performed on the dataset the results of which were similar to Bonferonni test.</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -432,7 +462,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -443,11 +473,11 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -480,6 +510,14 @@
     <font>
       <b/>
       <sz val="10.0"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
@@ -611,7 +649,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -621,23 +659,23 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -650,19 +688,19 @@
     <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
@@ -677,13 +715,13 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -692,7 +730,7 @@
     <xf borderId="0" fillId="0" fontId="8" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -713,12 +751,18 @@
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="11" numFmtId="11" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="11" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -734,11 +778,11 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="11" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -765,38 +809,38 @@
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="10" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="11" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="10" fillId="0" fontId="3" numFmtId="11" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="11" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -805,13 +849,19 @@
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -838,7 +888,7 @@
     <xdr:ext cx="7162800" cy="2609850"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -866,7 +916,7 @@
     <xdr:ext cx="7162800" cy="2609850"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -894,7 +944,7 @@
     <xdr:ext cx="7162800" cy="2609850"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -922,7 +972,7 @@
     <xdr:ext cx="7162800" cy="2609850"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -950,7 +1000,7 @@
     <xdr:ext cx="7162800" cy="2609850"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -978,7 +1028,7 @@
     <xdr:ext cx="7162800" cy="2609850"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -2031,25 +2081,25 @@
       <c r="Q6" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="R6" s="35">
+      <c r="R6" s="37">
         <v>-21.6667</v>
       </c>
-      <c r="S6" s="35">
+      <c r="S6" s="37">
         <v>0.001</v>
       </c>
-      <c r="T6" s="35">
+      <c r="T6" s="37">
         <v>-28.1169</v>
       </c>
-      <c r="U6" s="35">
+      <c r="U6" s="37">
         <v>-15.2164</v>
       </c>
       <c r="V6" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="W6" s="37"/>
-      <c r="X6" s="37"/>
-      <c r="Y6" s="37"/>
-      <c r="Z6" s="37"/>
+      <c r="W6" s="38"/>
+      <c r="X6" s="38"/>
+      <c r="Y6" s="38"/>
+      <c r="Z6" s="38"/>
     </row>
     <row r="7">
       <c r="A7" s="25">
@@ -2064,7 +2114,7 @@
       <c r="D7" s="26">
         <v>374.0</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="39" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="30">
@@ -2094,25 +2144,25 @@
       <c r="Q7" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="R7" s="35">
+      <c r="R7" s="40">
         <v>-6.5</v>
       </c>
-      <c r="S7" s="35">
+      <c r="S7" s="37">
         <v>0.0479</v>
       </c>
-      <c r="T7" s="35">
+      <c r="T7" s="37">
         <v>-12.9503</v>
       </c>
-      <c r="U7" s="35">
+      <c r="U7" s="37">
         <v>-0.0497</v>
       </c>
       <c r="V7" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="W7" s="37"/>
-      <c r="X7" s="37"/>
-      <c r="Y7" s="37"/>
-      <c r="Z7" s="37"/>
+      <c r="W7" s="38"/>
+      <c r="X7" s="38"/>
+      <c r="Y7" s="38"/>
+      <c r="Z7" s="38"/>
     </row>
     <row r="8">
       <c r="A8" s="25">
@@ -2127,7 +2177,7 @@
       <c r="D8" s="26">
         <v>310.0</v>
       </c>
-      <c r="F8" s="38">
+      <c r="F8" s="39">
         <v>0.25</v>
       </c>
       <c r="G8" s="30">
@@ -2145,28 +2195,28 @@
       <c r="P8" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="39" t="s">
+      <c r="Q8" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="R8" s="34">
+      <c r="R8" s="37">
         <v>15.1667</v>
       </c>
-      <c r="S8" s="35">
+      <c r="S8" s="37">
         <v>0.001</v>
       </c>
-      <c r="T8" s="35">
+      <c r="T8" s="37">
         <v>8.7164</v>
       </c>
-      <c r="U8" s="35">
+      <c r="U8" s="37">
         <v>21.6169</v>
       </c>
       <c r="V8" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="W8" s="37"/>
-      <c r="X8" s="37"/>
-      <c r="Y8" s="37"/>
-      <c r="Z8" s="37"/>
+      <c r="W8" s="38"/>
+      <c r="X8" s="38"/>
+      <c r="Y8" s="38"/>
+      <c r="Z8" s="38"/>
     </row>
     <row r="9">
       <c r="A9" s="25">
@@ -2181,7 +2231,7 @@
       <c r="D9" s="26">
         <v>414.0</v>
       </c>
-      <c r="F9" s="38">
+      <c r="F9" s="39">
         <v>0.5</v>
       </c>
       <c r="G9" s="30">
@@ -2196,10 +2246,10 @@
       <c r="K9" s="22"/>
       <c r="L9" s="22"/>
       <c r="M9" s="22"/>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="42"/>
-      <c r="S9" s="40"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="44"/>
+      <c r="S9" s="42"/>
     </row>
     <row r="10">
       <c r="A10" s="25">
@@ -2214,7 +2264,7 @@
       <c r="D10" s="26">
         <v>386.0</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="39">
         <v>0.75</v>
       </c>
       <c r="G10" s="30">
@@ -2250,7 +2300,7 @@
       <c r="D11" s="26">
         <v>366.0</v>
       </c>
-      <c r="F11" s="43" t="s">
+      <c r="F11" s="45" t="s">
         <v>37</v>
       </c>
       <c r="G11" s="30">
@@ -2310,25 +2360,25 @@
       <c r="Q12" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="R12" s="35">
+      <c r="R12" s="40">
         <v>-9.25</v>
       </c>
-      <c r="S12" s="35">
+      <c r="S12" s="37">
         <v>0.0078</v>
       </c>
-      <c r="T12" s="35">
+      <c r="T12" s="37">
         <v>-16.2868</v>
       </c>
-      <c r="U12" s="35">
+      <c r="U12" s="40">
         <v>-2.2132</v>
       </c>
       <c r="V12" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="W12" s="37"/>
-      <c r="X12" s="37"/>
-      <c r="Y12" s="37"/>
-      <c r="Z12" s="37"/>
+      <c r="W12" s="38"/>
+      <c r="X12" s="38"/>
+      <c r="Y12" s="38"/>
+      <c r="Z12" s="38"/>
     </row>
     <row r="13">
       <c r="A13" s="25">
@@ -2349,39 +2399,39 @@
       <c r="L13" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="M13" s="44" t="s">
+      <c r="M13" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="N13" s="45">
+      <c r="N13" s="47">
         <f> 0.05 / 3</f>
         <v>0.01666666667</v>
       </c>
-      <c r="O13" s="45"/>
+      <c r="O13" s="47"/>
       <c r="P13" s="36" t="s">
         <v>4</v>
       </c>
       <c r="Q13" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="R13" s="35">
+      <c r="R13" s="37">
         <v>-12.3333</v>
       </c>
-      <c r="S13" s="35">
+      <c r="S13" s="37">
         <v>0.001</v>
       </c>
-      <c r="T13" s="35">
+      <c r="T13" s="37">
         <v>-19.3702</v>
       </c>
-      <c r="U13" s="35">
+      <c r="U13" s="40">
         <v>-5.2965</v>
       </c>
       <c r="V13" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="W13" s="37"/>
-      <c r="X13" s="37"/>
-      <c r="Y13" s="37"/>
-      <c r="Z13" s="37"/>
+      <c r="W13" s="38"/>
+      <c r="X13" s="38"/>
+      <c r="Y13" s="38"/>
+      <c r="Z13" s="38"/>
     </row>
     <row r="14">
       <c r="A14" s="25">
@@ -2402,25 +2452,25 @@
       <c r="Q14" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="R14" s="34">
+      <c r="R14" s="40">
         <v>-3.0833</v>
       </c>
-      <c r="S14" s="35">
+      <c r="S14" s="37">
         <v>0.5351</v>
       </c>
-      <c r="T14" s="35">
+      <c r="T14" s="37">
         <v>-10.1202</v>
       </c>
-      <c r="U14" s="35">
+      <c r="U14" s="40">
         <v>3.9535</v>
       </c>
       <c r="V14" s="35" t="b">
         <v>0</v>
       </c>
-      <c r="W14" s="37"/>
-      <c r="X14" s="37"/>
-      <c r="Y14" s="37"/>
-      <c r="Z14" s="37"/>
+      <c r="W14" s="38"/>
+      <c r="X14" s="38"/>
+      <c r="Y14" s="38"/>
+      <c r="Z14" s="38"/>
     </row>
     <row r="15">
       <c r="K15" s="6" t="s">
@@ -2428,10 +2478,10 @@
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="2"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="41"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="40"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="44"/>
+      <c r="S15" s="42"/>
     </row>
     <row r="16">
       <c r="K16" s="1" t="s">
@@ -2441,7 +2491,7 @@
         <v>7</v>
       </c>
       <c r="M16" s="2"/>
-      <c r="N16" s="46"/>
+      <c r="N16" s="48"/>
       <c r="P16" s="2" t="s">
         <v>43</v>
       </c>
@@ -2458,7 +2508,7 @@
         <v>9</v>
       </c>
       <c r="M17" s="2"/>
-      <c r="N17" s="47"/>
+      <c r="N17" s="49"/>
       <c r="P17" s="32" t="s">
         <v>28</v>
       </c>
@@ -2502,32 +2552,32 @@
         <v>11</v>
       </c>
       <c r="M18" s="2"/>
-      <c r="N18" s="46"/>
+      <c r="N18" s="48"/>
       <c r="P18" s="36" t="s">
         <v>4</v>
       </c>
       <c r="Q18" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="R18" s="35">
+      <c r="R18" s="37">
         <v>-112.3333</v>
       </c>
-      <c r="S18" s="35">
+      <c r="S18" s="37">
         <v>0.001</v>
       </c>
-      <c r="T18" s="35">
+      <c r="T18" s="37">
         <v>-154.9302</v>
       </c>
-      <c r="U18" s="35">
+      <c r="U18" s="37">
         <v>-69.7365</v>
       </c>
       <c r="V18" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="W18" s="37"/>
-      <c r="X18" s="37"/>
-      <c r="Y18" s="37"/>
-      <c r="Z18" s="37"/>
+      <c r="W18" s="38"/>
+      <c r="X18" s="38"/>
+      <c r="Y18" s="38"/>
+      <c r="Z18" s="38"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
@@ -2549,25 +2599,25 @@
       <c r="Q19" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="R19" s="35">
+      <c r="R19" s="37">
         <v>-79.4167</v>
       </c>
-      <c r="S19" s="35">
+      <c r="S19" s="37">
         <v>0.001</v>
       </c>
-      <c r="T19" s="35">
+      <c r="T19" s="37">
         <v>-122.0135</v>
       </c>
-      <c r="U19" s="35">
+      <c r="U19" s="37">
         <v>-36.8198</v>
       </c>
       <c r="V19" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="W19" s="37"/>
-      <c r="X19" s="37"/>
-      <c r="Y19" s="37"/>
-      <c r="Z19" s="37"/>
+      <c r="W19" s="38"/>
+      <c r="X19" s="38"/>
+      <c r="Y19" s="38"/>
+      <c r="Z19" s="38"/>
     </row>
     <row r="20">
       <c r="A20" s="25">
@@ -2582,7 +2632,7 @@
       <c r="D20" s="26">
         <v>235.0</v>
       </c>
-      <c r="F20" s="48"/>
+      <c r="F20" s="50"/>
       <c r="G20" s="32" t="s">
         <v>20</v>
       </c>
@@ -2592,7 +2642,7 @@
       <c r="I20" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="K20" s="49" t="s">
+      <c r="K20" s="51" t="s">
         <v>48</v>
       </c>
       <c r="P20" s="36" t="s">
@@ -2601,25 +2651,25 @@
       <c r="Q20" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="R20" s="35">
+      <c r="R20" s="37">
         <v>32.9167</v>
       </c>
-      <c r="S20" s="35">
+      <c r="S20" s="37">
         <v>0.1559</v>
       </c>
-      <c r="T20" s="35">
+      <c r="T20" s="37">
         <v>-9.6802</v>
       </c>
-      <c r="U20" s="35">
+      <c r="U20" s="37">
         <v>75.5135</v>
       </c>
       <c r="V20" s="35" t="b">
         <v>0</v>
       </c>
-      <c r="W20" s="37"/>
-      <c r="X20" s="37"/>
-      <c r="Y20" s="37"/>
-      <c r="Z20" s="37"/>
+      <c r="W20" s="38"/>
+      <c r="X20" s="38"/>
+      <c r="Y20" s="38"/>
+      <c r="Z20" s="38"/>
     </row>
     <row r="21">
       <c r="A21" s="25">
@@ -2637,31 +2687,31 @@
       <c r="F21" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="50">
+      <c r="G21" s="52">
         <v>12.0</v>
       </c>
-      <c r="H21" s="50">
+      <c r="H21" s="52">
         <v>12.0</v>
       </c>
-      <c r="I21" s="50">
+      <c r="I21" s="52">
         <v>12.0</v>
       </c>
-      <c r="K21" s="51" t="s">
+      <c r="K21" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="L21" s="52" t="s">
+      <c r="L21" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="M21" s="53" t="s">
+      <c r="M21" s="55" t="s">
         <v>24</v>
       </c>
       <c r="N21" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="P21" s="40"/>
-      <c r="Q21" s="41"/>
-      <c r="R21" s="42"/>
-      <c r="S21" s="40"/>
+      <c r="P21" s="42"/>
+      <c r="Q21" s="43"/>
+      <c r="R21" s="44"/>
+      <c r="S21" s="42"/>
     </row>
     <row r="22">
       <c r="A22" s="25">
@@ -2679,33 +2729,33 @@
       <c r="F22" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="50">
+      <c r="G22" s="52">
         <v>64.0</v>
       </c>
-      <c r="H22" s="50">
+      <c r="H22" s="52">
         <v>31.1666666666667</v>
       </c>
-      <c r="I22" s="50">
+      <c r="I22" s="52">
         <v>280.083333333333</v>
       </c>
-      <c r="K22" s="54" t="s">
+      <c r="K22" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="L22" s="55">
+      <c r="L22" s="57">
         <v>2.71785852591474</v>
       </c>
-      <c r="M22" s="56">
+      <c r="M22" s="58">
         <v>0.012564279857587</v>
       </c>
-      <c r="N22" s="57" t="b">
+      <c r="N22" s="59" t="b">
         <v>1</v>
       </c>
       <c r="P22" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="Q22" s="41"/>
-      <c r="R22" s="42"/>
-      <c r="S22" s="40"/>
+      <c r="Q22" s="43"/>
+      <c r="R22" s="44"/>
+      <c r="S22" s="42"/>
     </row>
     <row r="23">
       <c r="A23" s="25">
@@ -2723,31 +2773,31 @@
       <c r="F23" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="50">
+      <c r="G23" s="52">
         <v>6.09023062707063</v>
       </c>
-      <c r="H23" s="50">
+      <c r="H23" s="52">
         <v>8.57939745005794</v>
       </c>
-      <c r="I23" s="50">
+      <c r="I23" s="52">
         <v>49.0703730895896</v>
       </c>
-      <c r="K23" s="54" t="s">
+      <c r="K23" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="L23" s="55">
+      <c r="L23" s="57">
         <v>8.0314268217978</v>
       </c>
-      <c r="M23" s="56">
+      <c r="M23" s="58">
         <v>5.53092858862259E-8</v>
       </c>
-      <c r="N23" s="57" t="b">
+      <c r="N23" s="59" t="b">
         <v>1</v>
       </c>
-      <c r="P23" s="40"/>
-      <c r="Q23" s="41"/>
-      <c r="R23" s="42"/>
-      <c r="S23" s="40"/>
+      <c r="P23" s="42"/>
+      <c r="Q23" s="43"/>
+      <c r="R23" s="44"/>
+      <c r="S23" s="42"/>
     </row>
     <row r="24">
       <c r="A24" s="25">
@@ -2765,25 +2815,25 @@
       <c r="F24" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="50">
+      <c r="G24" s="52">
         <v>58.0</v>
       </c>
-      <c r="H24" s="50">
+      <c r="H24" s="52">
         <v>21.0</v>
       </c>
-      <c r="I24" s="50">
+      <c r="I24" s="52">
         <v>207.0</v>
       </c>
-      <c r="K24" s="58" t="s">
+      <c r="K24" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="L24" s="55">
+      <c r="L24" s="57">
         <v>5.45158132917237</v>
       </c>
-      <c r="M24" s="56">
+      <c r="M24" s="58">
         <v>1.77815781034481E-5</v>
       </c>
-      <c r="N24" s="59" t="b">
+      <c r="N24" s="61" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2800,22 +2850,22 @@
       <c r="D25" s="26">
         <v>250.0</v>
       </c>
-      <c r="F25" s="60">
+      <c r="F25" s="62">
         <v>0.25</v>
       </c>
-      <c r="G25" s="50">
+      <c r="G25" s="52">
         <v>58.0</v>
       </c>
-      <c r="H25" s="50">
+      <c r="H25" s="52">
         <v>26.75</v>
       </c>
-      <c r="I25" s="50">
+      <c r="I25" s="52">
         <v>249.75</v>
       </c>
-      <c r="K25" s="61"/>
-      <c r="L25" s="61"/>
-      <c r="M25" s="61"/>
-      <c r="N25" s="61"/>
+      <c r="K25" s="63"/>
+      <c r="L25" s="63"/>
+      <c r="M25" s="63"/>
+      <c r="N25" s="63"/>
     </row>
     <row r="26">
       <c r="A26" s="25">
@@ -2830,24 +2880,24 @@
       <c r="D26" s="26">
         <v>293.0</v>
       </c>
-      <c r="F26" s="60">
+      <c r="F26" s="62">
         <v>0.5</v>
       </c>
-      <c r="G26" s="50">
+      <c r="G26" s="52">
         <v>62.5</v>
       </c>
-      <c r="H26" s="50">
+      <c r="H26" s="52">
         <v>28.5</v>
       </c>
-      <c r="I26" s="50">
+      <c r="I26" s="52">
         <v>273.5</v>
       </c>
-      <c r="K26" s="62" t="s">
+      <c r="K26" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="L26" s="63"/>
-      <c r="M26" s="63"/>
-      <c r="N26" s="63"/>
+      <c r="L26" s="65"/>
+      <c r="M26" s="65"/>
+      <c r="N26" s="65"/>
     </row>
     <row r="27">
       <c r="A27" s="25">
@@ -2862,25 +2912,25 @@
       <c r="D27" s="26">
         <v>260.0</v>
       </c>
-      <c r="F27" s="60">
+      <c r="F27" s="62">
         <v>0.75</v>
       </c>
-      <c r="G27" s="50">
+      <c r="G27" s="52">
         <v>70.0</v>
       </c>
-      <c r="H27" s="50">
+      <c r="H27" s="52">
         <v>31.25</v>
       </c>
-      <c r="I27" s="50">
+      <c r="I27" s="52">
         <v>299.25</v>
       </c>
-      <c r="K27" s="54" t="s">
+      <c r="K27" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="L27" s="64" t="s">
+      <c r="L27" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="M27" s="65" t="s">
+      <c r="M27" s="67" t="s">
         <v>24</v>
       </c>
       <c r="N27" s="33" t="s">
@@ -2903,25 +2953,25 @@
       <c r="F28" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="G28" s="50">
+      <c r="G28" s="52">
         <v>72.0</v>
       </c>
-      <c r="H28" s="50">
+      <c r="H28" s="52">
         <v>52.0</v>
       </c>
-      <c r="I28" s="50">
+      <c r="I28" s="52">
         <v>394.0</v>
       </c>
-      <c r="K28" s="54" t="s">
+      <c r="K28" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="L28" s="55">
+      <c r="L28" s="57">
         <v>4.1809062157238</v>
       </c>
-      <c r="M28" s="56">
+      <c r="M28" s="58">
         <v>3.87874830903E-4</v>
       </c>
-      <c r="N28" s="57" t="b">
+      <c r="N28" s="59" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2938,16 +2988,16 @@
       <c r="D29" s="26">
         <v>265.0</v>
       </c>
-      <c r="K29" s="54" t="s">
+      <c r="K29" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="L29" s="55">
+      <c r="L29" s="57">
         <v>3.71296173339954</v>
       </c>
-      <c r="M29" s="56">
+      <c r="M29" s="58">
         <v>0.001211479431689</v>
       </c>
-      <c r="N29" s="57" t="b">
+      <c r="N29" s="59" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2964,16 +3014,16 @@
       <c r="D30" s="26">
         <v>394.0</v>
       </c>
-      <c r="K30" s="58" t="s">
+      <c r="K30" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="L30" s="55">
+      <c r="L30" s="57">
         <v>-0.986339933411334</v>
       </c>
-      <c r="M30" s="56">
+      <c r="M30" s="58">
         <v>0.334690659752219</v>
       </c>
-      <c r="N30" s="59" t="b">
+      <c r="N30" s="61" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2990,33 +3040,33 @@
       <c r="D31" s="26">
         <v>282.0</v>
       </c>
-      <c r="K31" s="66"/>
-      <c r="L31" s="66"/>
-      <c r="M31" s="66"/>
-      <c r="N31" s="66"/>
+      <c r="K31" s="68"/>
+      <c r="L31" s="68"/>
+      <c r="M31" s="68"/>
+      <c r="N31" s="68"/>
     </row>
     <row r="32">
-      <c r="K32" s="61"/>
-      <c r="L32" s="61"/>
-      <c r="M32" s="61"/>
-      <c r="N32" s="61"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="63"/>
     </row>
     <row r="33">
-      <c r="K33" s="62" t="s">
+      <c r="K33" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="L33" s="63"/>
-      <c r="M33" s="63"/>
-      <c r="N33" s="63"/>
+      <c r="L33" s="65"/>
+      <c r="M33" s="65"/>
+      <c r="N33" s="65"/>
     </row>
     <row r="34">
-      <c r="K34" s="54" t="s">
+      <c r="K34" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="L34" s="67" t="s">
+      <c r="L34" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="M34" s="65" t="s">
+      <c r="M34" s="67" t="s">
         <v>24</v>
       </c>
       <c r="N34" s="33" t="s">
@@ -3033,16 +3083,16 @@
       <c r="F35" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K35" s="54" t="s">
+      <c r="K35" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="L35" s="55">
+      <c r="L35" s="57">
         <v>4.1809062157238</v>
       </c>
-      <c r="M35" s="56">
+      <c r="M35" s="58">
         <v>3.87874830903E-4</v>
       </c>
-      <c r="N35" s="57" t="b">
+      <c r="N35" s="59" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3059,16 +3109,16 @@
       <c r="D36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K36" s="54" t="s">
+      <c r="K36" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="L36" s="55">
+      <c r="L36" s="57">
         <v>3.71296173339954</v>
       </c>
-      <c r="M36" s="56">
+      <c r="M36" s="58">
         <v>0.001211479431689</v>
       </c>
-      <c r="N36" s="57" t="b">
+      <c r="N36" s="59" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3085,7 +3135,7 @@
       <c r="D37" s="26">
         <v>227.0</v>
       </c>
-      <c r="F37" s="68"/>
+      <c r="F37" s="70"/>
       <c r="G37" s="32" t="s">
         <v>20</v>
       </c>
@@ -3095,16 +3145,16 @@
       <c r="I37" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="K37" s="58" t="s">
+      <c r="K37" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="L37" s="55">
+      <c r="L37" s="57">
         <v>-0.986339933411334</v>
       </c>
-      <c r="M37" s="56">
+      <c r="M37" s="58">
         <v>0.334690659752219</v>
       </c>
-      <c r="N37" s="59" t="b">
+      <c r="N37" s="61" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3124,13 +3174,13 @@
       <c r="F38" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="G38" s="50">
+      <c r="G38" s="52">
         <v>12.0</v>
       </c>
-      <c r="H38" s="50">
+      <c r="H38" s="52">
         <v>12.0</v>
       </c>
-      <c r="I38" s="50">
+      <c r="I38" s="52">
         <v>12.0</v>
       </c>
     </row>
@@ -3150,14 +3200,17 @@
       <c r="F39" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="G39" s="50">
+      <c r="G39" s="52">
         <v>48.8333333333333</v>
       </c>
-      <c r="H39" s="50">
+      <c r="H39" s="52">
         <v>34.25</v>
       </c>
-      <c r="I39" s="50">
+      <c r="I39" s="52">
         <v>247.166666666667</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="40">
@@ -3176,14 +3229,17 @@
       <c r="F40" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="G40" s="50">
+      <c r="G40" s="52">
         <v>7.46912838207235</v>
       </c>
-      <c r="H40" s="50">
+      <c r="H40" s="52">
         <v>6.60750262270783</v>
       </c>
-      <c r="I40" s="50">
+      <c r="I40" s="52">
         <v>37.8125360004837</v>
+      </c>
+      <c r="K40" s="71" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="41">
@@ -3202,13 +3258,13 @@
       <c r="F41" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="G41" s="50">
+      <c r="G41" s="52">
         <v>36.0</v>
       </c>
-      <c r="H41" s="50">
+      <c r="H41" s="52">
         <v>23.0</v>
       </c>
-      <c r="I41" s="50">
+      <c r="I41" s="52">
         <v>192.0</v>
       </c>
     </row>
@@ -3225,16 +3281,16 @@
       <c r="D42" s="26">
         <v>192.0</v>
       </c>
-      <c r="F42" s="60">
+      <c r="F42" s="62">
         <v>0.25</v>
       </c>
-      <c r="G42" s="50">
+      <c r="G42" s="52">
         <v>44.75</v>
       </c>
-      <c r="H42" s="50">
+      <c r="H42" s="52">
         <v>29.0</v>
       </c>
-      <c r="I42" s="50">
+      <c r="I42" s="52">
         <v>224.25</v>
       </c>
     </row>
@@ -3251,16 +3307,16 @@
       <c r="D43" s="26">
         <v>275.0</v>
       </c>
-      <c r="F43" s="60">
+      <c r="F43" s="62">
         <v>0.5</v>
       </c>
-      <c r="G43" s="50">
+      <c r="G43" s="52">
         <v>47.5</v>
       </c>
-      <c r="H43" s="50">
+      <c r="H43" s="52">
         <v>37.0</v>
       </c>
-      <c r="I43" s="50">
+      <c r="I43" s="52">
         <v>240.0</v>
       </c>
     </row>
@@ -3277,16 +3333,16 @@
       <c r="D44" s="26">
         <v>244.0</v>
       </c>
-      <c r="F44" s="60">
+      <c r="F44" s="62">
         <v>0.75</v>
       </c>
-      <c r="G44" s="50">
+      <c r="G44" s="52">
         <v>52.25</v>
       </c>
-      <c r="H44" s="50">
+      <c r="H44" s="52">
         <v>39.0</v>
       </c>
-      <c r="I44" s="50">
+      <c r="I44" s="52">
         <v>275.25</v>
       </c>
     </row>
@@ -3306,13 +3362,13 @@
       <c r="F45" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="G45" s="50">
+      <c r="G45" s="52">
         <v>64.0</v>
       </c>
-      <c r="H45" s="50">
+      <c r="H45" s="52">
         <v>42.0</v>
       </c>
-      <c r="I45" s="50">
+      <c r="I45" s="52">
         <v>326.0</v>
       </c>
     </row>
@@ -3360,58 +3416,102 @@
     </row>
     <row r="50">
       <c r="H50" s="22"/>
+      <c r="K50" s="72"/>
+      <c r="L50" s="72"/>
+      <c r="M50" s="72"/>
+      <c r="N50" s="72"/>
     </row>
     <row r="51">
       <c r="F51" s="29"/>
       <c r="G51" s="29"/>
       <c r="H51" s="22"/>
+      <c r="K51" s="72"/>
+      <c r="L51" s="72"/>
+      <c r="M51" s="72"/>
+      <c r="N51" s="72"/>
     </row>
     <row r="52">
       <c r="A52" s="29"/>
       <c r="B52" s="29"/>
       <c r="F52" s="29"/>
-      <c r="G52" s="69"/>
+      <c r="G52" s="73"/>
       <c r="H52" s="22"/>
+      <c r="K52" s="72"/>
+      <c r="L52" s="72"/>
+      <c r="M52" s="72"/>
+      <c r="N52" s="72"/>
     </row>
     <row r="53">
       <c r="A53" s="29"/>
-      <c r="B53" s="69"/>
+      <c r="B53" s="73"/>
       <c r="F53" s="29"/>
-      <c r="G53" s="69"/>
+      <c r="G53" s="73"/>
       <c r="H53" s="22"/>
+      <c r="K53" s="72"/>
+      <c r="L53" s="72"/>
+      <c r="M53" s="72"/>
+      <c r="N53" s="72"/>
     </row>
     <row r="54">
       <c r="A54" s="29"/>
-      <c r="B54" s="69"/>
+      <c r="B54" s="73"/>
       <c r="F54" s="29"/>
-      <c r="G54" s="69"/>
+      <c r="G54" s="73"/>
       <c r="H54" s="22"/>
+      <c r="K54" s="72"/>
+      <c r="L54" s="72"/>
+      <c r="M54" s="72"/>
+      <c r="N54" s="72"/>
     </row>
     <row r="55">
       <c r="A55" s="29"/>
-      <c r="B55" s="69"/>
+      <c r="B55" s="73"/>
       <c r="F55" s="22"/>
       <c r="G55" s="22"/>
       <c r="H55" s="22"/>
+      <c r="K55" s="72"/>
+      <c r="L55" s="72"/>
+      <c r="M55" s="72"/>
+      <c r="N55" s="72"/>
     </row>
     <row r="56">
       <c r="F56" s="22"/>
       <c r="G56" s="22"/>
       <c r="H56" s="22"/>
+      <c r="K56" s="72"/>
+      <c r="L56" s="72"/>
+      <c r="M56" s="72"/>
+      <c r="N56" s="72"/>
     </row>
     <row r="57">
       <c r="F57" s="22"/>
       <c r="G57" s="22"/>
       <c r="H57" s="22"/>
+      <c r="K57" s="72"/>
+      <c r="L57" s="72"/>
+      <c r="M57" s="72"/>
+      <c r="N57" s="72"/>
+    </row>
+    <row r="58">
+      <c r="K58" s="72"/>
+      <c r="L58" s="72"/>
+      <c r="M58" s="72"/>
+      <c r="N58" s="72"/>
+    </row>
+    <row r="59">
+      <c r="K59" s="72"/>
+      <c r="L59" s="72"/>
+      <c r="M59" s="72"/>
+      <c r="N59" s="72"/>
     </row>
     <row r="67">
-      <c r="P67" s="70" t="s">
-        <v>59</v>
-      </c>
-      <c r="S67" s="71"/>
+      <c r="P67" s="74" t="s">
+        <v>61</v>
+      </c>
+      <c r="S67" s="75"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="20">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="K2:L2"/>
@@ -3424,6 +3524,7 @@
     <mergeCell ref="K33:N33"/>
     <mergeCell ref="A35:D35"/>
     <mergeCell ref="F35:I35"/>
+    <mergeCell ref="K40:N49"/>
     <mergeCell ref="K11:N11"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="M15:N15"/>

</xml_diff>